<commit_message>
fix: Modifies a majority of Skills entity with DTO and Test to ensure compatibility with the Frontend
</commit_message>
<xml_diff>
--- a/src/main/resources/data/test-skills.xlsx
+++ b/src/main/resources/data/test-skills.xlsx
@@ -53,15 +53,9 @@
     <t>BUFF</t>
   </si>
   <si>
-    <t>OFFENSIVE</t>
-  </si>
-  <si>
     <t>INNATE</t>
   </si>
   <si>
-    <t>BUFF, OFFENSIVE</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
@@ -123,6 +117,12 @@
   </si>
   <si>
     <t>hero2_EG</t>
+  </si>
+  <si>
+    <t>DAMAGE</t>
+  </si>
+  <si>
+    <t>BUFF, DAMAGE</t>
   </si>
 </sst>
 </file>
@@ -480,7 +480,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -521,103 +521,103 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" t="s">
         <v>31</v>
-      </c>
-      <c r="H3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C4">
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H4" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C5">
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H5" t="s">
         <v>8</v>
@@ -625,158 +625,158 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C6">
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H6" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H8" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C9">
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H9" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C10">
         <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H10" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C11">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H11" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>